<commit_message>
patch 1.12 | oprava responzivity pri navigacii
</commit_message>
<xml_diff>
--- a/public/vyrobkyUNF.xlsx
+++ b/public/vyrobkyUNF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\Webiky\tpv-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA3CC45-D51D-468B-9167-A826240630E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E3E8F3-23D4-4997-B3AB-CF0E6AD63F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="525" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diel" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>99-23-3426</t>
   </si>
@@ -123,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,6 +133,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,7 +444,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -485,13 +488,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1">
@@ -506,20 +509,14 @@
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1">
         <v>2</v>
       </c>
@@ -532,20 +529,12 @@
       <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="1">
         <v>3</v>
       </c>
@@ -563,13 +552,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1">
@@ -584,20 +573,14 @@
       <c r="G5" s="1">
         <v>5</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1">
         <v>2</v>
       </c>
@@ -610,11 +593,19 @@
       <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C6"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>